<commit_message>
optimize data and new function for UAT
</commit_message>
<xml_diff>
--- a/resource/eor/EORLRScoreTemplate.xlsx
+++ b/resource/eor/EORLRScoreTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20610" windowHeight="8730"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Test Centre</t>
   </si>
@@ -42,44 +42,18 @@
   <si>
     <t xml:space="preserve">EOR L/R Score Input sheet 
                                          </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test Details</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Test date</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Shijiazhuang	</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">6.0	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yyyy-mm-dd	</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hello Kitty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-West Region	</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -96,16 +70,25 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>005774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Region	</t>
+  </si>
+  <si>
+    <t>BJ-UIBE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -114,12 +97,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -241,30 +218,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -273,32 +250,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -311,7 +291,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -600,32 +580,32 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="12" customWidth="1"/>
-    <col min="2" max="3" width="12.375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.25" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="12"/>
+    <col min="1" max="1" width="14" style="8" customWidth="1"/>
+    <col min="2" max="3" width="12.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
@@ -638,18 +618,18 @@
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -679,28 +659,28 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5">
+        <v>42760</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="15">
+        <v>990801</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6">
-        <v>123456</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>12</v>
+      <c r="H5" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>